<commit_message>
Fixing the naming of variables in the documentation & code
</commit_message>
<xml_diff>
--- a/Specification/PIF Format Specification.xlsx
+++ b/Specification/PIF Format Specification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a3e342190b4c8ac1/Dokumente/Programmieren/vs_code/EmbeddedImageFormat/Specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="13_ncr:4000b_{7BD3CF34-DE1A-416A-B684-A949E09A7977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{872F22C3-F1A4-4B1C-BA81-165A71617966}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:4000b_{7BD3CF34-DE1A-416A-B684-A949E09A7977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9895AF5C-2762-49CA-A9F5-C4014C702144}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16749" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIF Format Specification" sheetId="1" r:id="rId1"/>
@@ -64,26 +64,6 @@
     <t>File Offset to PixelArray</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t>Note</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t>: The size of the File
-and Image header are fixed</t>
-    </r>
-  </si>
-  <si>
     <t>Image Information Header</t>
   </si>
   <si>
@@ -91,29 +71,6 @@
   </si>
   <si>
     <t>Bits per Pixel</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t>Note</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t>: The presence of the
-Color Table is mandatory
-when Bits per Pixel ≤ 8,
-unless Image Type states
-RGB332, RGB16C or B/W</t>
-    </r>
   </si>
   <si>
     <t>Image Type:</t>
@@ -461,6 +418,45 @@
     <t>Indexed Colors, RGB332 per Index</t>
   </si>
   <si>
+    <t>Blue n-1</t>
+  </si>
+  <si>
+    <t>Pixel[w-2,0]</t>
+  </si>
+  <si>
+    <t>Pixel[w-2,1]</t>
+  </si>
+  <si>
+    <t>Pixel[w-2,2]</t>
+  </si>
+  <si>
+    <t>Pixel[w-2,h-2]</t>
+  </si>
+  <si>
+    <t>Pixel[w-2,h-1]</t>
+  </si>
+  <si>
+    <t>Raw 24-bit image data</t>
+  </si>
+  <si>
+    <t>16 color mode with fixed Windows/IBM Colors*</t>
+  </si>
+  <si>
+    <t>Bit size that each Pixel occupies. Bit size for an Indexed Image cannot go beyond 8 bits.</t>
+  </si>
+  <si>
+    <t>Size of the (compressed) image data in Bytes</t>
+  </si>
+  <si>
+    <t>The Color Data in the table is either RGB888, RGB565 or RGB332. The amount of Colors has to be same or less than the [Bits per Pixel] allow, otherwise the image is invalid. If data refers to a higher index number than the Color Table holds, the image is also invalid.</t>
+  </si>
+  <si>
+    <t>To identify a valid .PIF file. The signature is ‹PIF› as string, including null character: {'P','I','F','\0'}</t>
+  </si>
+  <si>
+    <t>Size of the color table in bytes, only used in Indexed mode, otherwise zero.</t>
+  </si>
+  <si>
     <r>
       <t>Note</t>
     </r>
@@ -470,12 +466,56 @@
         <rFont val="DejaVu Sans"/>
         <family val="2"/>
       </rPr>
-      <t>: The size of the Color
-Table Entries depends on the selected Index Image Type. Possible sizes are 3 bytes, 2 bytes or one byte per color.</t>
-    </r>
-  </si>
-  <si>
-    <t>Blue n-1</t>
+      <t xml:space="preserve">: While </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>ColorTableSize</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> states the amount of bytes in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>ColorTable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>ImageType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> states how many bytes make up a color.</t>
+    </r>
   </si>
   <si>
     <r>
@@ -487,56 +527,155 @@
         <rFont val="DejaVu Sans"/>
         <family val="2"/>
       </rPr>
-      <t>: Pixel size depending on
-[Bits per Pixel] field. If Bits per 
-Pixel is ≤ 4, multiple Pixels
+      <t xml:space="preserve">: The presence of the
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>ColorTable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> is mandatory
+when Bits per Pixel ≤ 8,
+unless </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>ImageType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> states
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>RGB332</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>RGB16C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>B/W</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>: The size of the File
+and Image Header are fixed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: Pixel size depending on
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>Bits per Pixel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> field. If </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>Bits per 
+Pixel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> is ≤ 4, multiple Pixels
 are grouped in one Byte
-but are not allowed to overlap
+and are not allowed to overlap
 the byte / 8-bit boundary.</t>
     </r>
-  </si>
-  <si>
-    <t>Pixel[w-2,0]</t>
-  </si>
-  <si>
-    <t>Pixel[w-2,1]</t>
-  </si>
-  <si>
-    <t>Pixel[w-2,2]</t>
-  </si>
-  <si>
-    <t>Pixel[w-2,h-2]</t>
-  </si>
-  <si>
-    <t>Pixel[w-2,h-1]</t>
-  </si>
-  <si>
-    <t>Raw 24-bit image data</t>
-  </si>
-  <si>
-    <t>16 color mode with fixed Windows/IBM Colors*</t>
-  </si>
-  <si>
-    <t>Bit size that each Pixel occupies. Bit size for an Indexed Image cannot go beyond 8 bits.</t>
-  </si>
-  <si>
-    <t>Size of the (compressed) image data in Bytes</t>
-  </si>
-  <si>
-    <t>Index size of the color table, only used in Indexed mode, otherwise zero.</t>
-  </si>
-  <si>
-    <t>The Color Data in the table is either RGB888, RGB565 or RGB332. The amount of Colors has to be same or less than the [Bits per Pixel] allow, otherwise the image is invalid. If data refers to a higher index number than the Color Table holds, the image is also invalid.</t>
-  </si>
-  <si>
-    <t>To identify a valid .PIF file. The signature is ‹PIF› as string, including null character: {'P','I','F','\0'}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="DejaVu Sans"/>
@@ -569,6 +708,11 @@
       <color theme="0"/>
       <name val="DejaVu Sans"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="DejaVu Sans"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1005,11 +1149,119 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1065,9 +1317,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1076,111 +1325,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1265,6 +1409,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1625,130 +1773,130 @@
   <dimension ref="B1:V69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:P5"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="12.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="6" max="6" width="3.84375" customWidth="1"/>
-    <col min="7" max="8" width="12.53515625" customWidth="1"/>
-    <col min="9" max="9" width="6.3046875" customWidth="1"/>
-    <col min="10" max="10" width="8.69140625" customWidth="1"/>
-    <col min="11" max="11" width="12.3046875" customWidth="1"/>
-    <col min="12" max="12" width="9.84375" customWidth="1"/>
-    <col min="16" max="16" width="11.53515625" customWidth="1"/>
-    <col min="17" max="17" width="8.69140625" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" customWidth="1"/>
+    <col min="7" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="12.9" thickBot="1">
+    <row r="1" spans="2:22" ht="13.5" thickBot="1">
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="2:22" ht="13.3" thickTop="1" thickBot="1">
+    <row r="2" spans="2:22" ht="14.25" thickTop="1" thickBot="1">
       <c r="G2" s="1"/>
-      <c r="K2" s="76" t="s">
+      <c r="K2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
-      <c r="P2" s="76"/>
-    </row>
-    <row r="3" spans="2:22" ht="13.3" thickTop="1" thickBot="1">
-      <c r="B3" s="68" t="s">
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+    </row>
+    <row r="3" spans="2:22" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="26" t="s">
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="76"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="76"/>
-    </row>
-    <row r="4" spans="2:22" ht="12.9" thickTop="1">
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="K4" s="69" t="s">
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+    </row>
+    <row r="4" spans="2:22" ht="13.5" thickTop="1">
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="K4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="77" t="s">
-        <v>121</v>
-      </c>
-      <c r="M4" s="77"/>
-      <c r="N4" s="77"/>
-      <c r="O4" s="77"/>
-      <c r="P4" s="78"/>
+      <c r="L4" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="30"/>
     </row>
     <row r="5" spans="2:22">
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
-      <c r="N5" s="79"/>
-      <c r="O5" s="79"/>
-      <c r="P5" s="80"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="32"/>
     </row>
     <row r="6" spans="2:22" ht="12.75" customHeight="1">
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="K6" s="69" t="s">
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="K6" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="L6" s="71" t="s">
+      <c r="L6" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="71"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="71"/>
-      <c r="P6" s="72"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="41"/>
       <c r="T6" s="21"/>
       <c r="U6" s="21"/>
       <c r="V6" s="21"/>
     </row>
     <row r="7" spans="2:22" ht="12.75" customHeight="1" thickBot="1">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="K7" s="70"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="73"/>
-      <c r="N7" s="73"/>
-      <c r="O7" s="73"/>
-      <c r="P7" s="74"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="43"/>
       <c r="T7" s="21"/>
       <c r="U7" s="21"/>
       <c r="V7" s="21"/>
@@ -1758,136 +1906,136 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="K8" s="63" t="s">
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="K8" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="63"/>
-      <c r="M8" s="64" t="s">
+      <c r="L8" s="46"/>
+      <c r="M8" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="N8" s="64"/>
-      <c r="O8" s="64"/>
-      <c r="P8" s="64"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="47"/>
       <c r="T8" s="21"/>
       <c r="U8" s="21"/>
       <c r="V8" s="21"/>
     </row>
-    <row r="9" spans="2:22" ht="13.3" thickTop="1" thickBot="1">
-      <c r="B9" s="66" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="63"/>
-      <c r="M9" s="64"/>
-      <c r="N9" s="64"/>
-      <c r="O9" s="64"/>
-      <c r="P9" s="64"/>
+    <row r="9" spans="2:22" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B9" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
+      <c r="P9" s="47"/>
       <c r="T9" s="21"/>
       <c r="U9" s="21"/>
       <c r="V9" s="21"/>
     </row>
     <row r="10" spans="2:22" ht="12.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B10" s="66"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
       <c r="T10" s="21"/>
       <c r="U10" s="21"/>
       <c r="V10" s="21"/>
     </row>
-    <row r="11" spans="2:22" ht="13.3" thickTop="1" thickBot="1">
-      <c r="B11" s="55" t="s">
+    <row r="11" spans="2:22" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B11" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="52"/>
+      <c r="D11" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="55"/>
-      <c r="D11" s="56" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="56"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="K11" s="67" t="s">
-        <v>11</v>
-      </c>
-      <c r="L11" s="67"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="67"/>
-      <c r="O11" s="67"/>
-      <c r="P11" s="67"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="K11" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="50"/>
+      <c r="P11" s="50"/>
       <c r="T11" s="21"/>
       <c r="U11" s="21"/>
       <c r="V11" s="21"/>
     </row>
     <row r="12" spans="2:22" ht="12.75" customHeight="1" thickTop="1">
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="52"/>
+      <c r="D12" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="53"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+    </row>
+    <row r="13" spans="2:22">
+      <c r="B13" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="55"/>
-      <c r="D12" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="56"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="67"/>
-      <c r="M12" s="67"/>
-      <c r="N12" s="67"/>
-      <c r="O12" s="67"/>
-      <c r="P12" s="67"/>
-    </row>
-    <row r="13" spans="2:22">
-      <c r="B13" s="59" t="s">
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="K13" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="M13" s="55"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="55"/>
+      <c r="P13" s="55"/>
+    </row>
+    <row r="14" spans="2:22" ht="13.5" thickBot="1">
+      <c r="B14" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="K13" s="57" t="s">
-        <v>15</v>
-      </c>
-      <c r="L13" s="58" t="s">
-        <v>16</v>
-      </c>
-      <c r="M13" s="58"/>
-      <c r="N13" s="58"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="58"/>
-    </row>
-    <row r="14" spans="2:22" ht="12.9" thickBot="1">
-      <c r="B14" s="60" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="60"/>
-      <c r="D14" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="61"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="58"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="58"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="58"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="58"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="55"/>
+      <c r="M14" s="55"/>
+      <c r="N14" s="55"/>
+      <c r="O14" s="55"/>
+      <c r="P14" s="55"/>
       <c r="S14" s="21"/>
       <c r="T14" s="21"/>
       <c r="U14" s="21"/>
@@ -1900,278 +2048,278 @@
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
-      <c r="K15" s="50" t="s">
-        <v>20</v>
-      </c>
-      <c r="L15" s="50"/>
-      <c r="M15" s="51" t="s">
-        <v>115</v>
-      </c>
-      <c r="N15" s="51"/>
-      <c r="O15" s="51"/>
-      <c r="P15" s="51"/>
+      <c r="K15" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="33"/>
+      <c r="M15" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
       <c r="S15" s="21"/>
       <c r="T15" s="21"/>
       <c r="U15" s="21"/>
     </row>
-    <row r="16" spans="2:22" ht="13.3" thickTop="1" thickBot="1">
-      <c r="B16" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="K16" s="50" t="s">
-        <v>23</v>
-      </c>
-      <c r="L16" s="50"/>
-      <c r="M16" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="N16" s="51"/>
-      <c r="O16" s="51"/>
-      <c r="P16" s="51"/>
+    <row r="16" spans="2:22" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B16" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="K16" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="33"/>
+      <c r="M16" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
       <c r="S16" s="21"/>
       <c r="T16" s="21"/>
       <c r="U16" s="21"/>
     </row>
-    <row r="17" spans="2:21" ht="12.9" thickTop="1">
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="K17" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="L17" s="50"/>
-      <c r="M17" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="N17" s="51"/>
-      <c r="O17" s="51"/>
-      <c r="P17" s="51"/>
+    <row r="17" spans="2:21" ht="13.5" thickTop="1">
+      <c r="B17" s="62"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="K17" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" s="33"/>
+      <c r="M17" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
       <c r="S17" s="21"/>
       <c r="T17" s="21"/>
       <c r="U17" s="21"/>
     </row>
     <row r="18" spans="2:21">
       <c r="B18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="E18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="K18" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="L18" s="50"/>
-      <c r="M18" s="51" t="s">
-        <v>116</v>
-      </c>
-      <c r="N18" s="51"/>
-      <c r="O18" s="51"/>
-      <c r="P18" s="51"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="K18" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="33"/>
+      <c r="M18" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
       <c r="S18" s="21"/>
       <c r="T18" s="21"/>
       <c r="U18" s="21"/>
     </row>
     <row r="19" spans="2:21">
       <c r="B19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="E19" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="K19" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="L19" s="50"/>
-      <c r="M19" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="N19" s="51"/>
-      <c r="O19" s="51"/>
-      <c r="P19" s="51"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="K19" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" s="33"/>
+      <c r="M19" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
       <c r="S19" s="21"/>
       <c r="T19" s="21"/>
       <c r="U19" s="21"/>
     </row>
     <row r="20" spans="2:21">
       <c r="B20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="E20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="K20" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="L20" s="33"/>
+      <c r="M20" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="34"/>
+    </row>
+    <row r="21" spans="2:21" ht="12.75" customHeight="1">
+      <c r="B21" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="K20" s="50" t="s">
-        <v>101</v>
-      </c>
-      <c r="L20" s="50"/>
-      <c r="M20" s="51" t="s">
-        <v>104</v>
-      </c>
-      <c r="N20" s="51"/>
-      <c r="O20" s="51"/>
-      <c r="P20" s="51"/>
-    </row>
-    <row r="21" spans="2:21" ht="12.75" customHeight="1">
-      <c r="B21" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="K21" s="50" t="s">
-        <v>102</v>
-      </c>
-      <c r="L21" s="50"/>
-      <c r="M21" s="51" t="s">
-        <v>105</v>
-      </c>
-      <c r="N21" s="51"/>
-      <c r="O21" s="51"/>
-      <c r="P21" s="51"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="K21" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="L21" s="33"/>
+      <c r="M21" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
     </row>
     <row r="22" spans="2:21">
-      <c r="B22" s="53"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
       <c r="F22" s="21"/>
       <c r="G22" s="21"/>
       <c r="H22" s="21"/>
-      <c r="K22" s="81" t="s">
-        <v>103</v>
-      </c>
-      <c r="L22" s="81"/>
-      <c r="M22" s="82" t="s">
-        <v>106</v>
-      </c>
-      <c r="N22" s="82"/>
-      <c r="O22" s="82"/>
-      <c r="P22" s="82"/>
+      <c r="K22" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="L22" s="35"/>
+      <c r="M22" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
     </row>
     <row r="23" spans="2:21" ht="12.75" customHeight="1">
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="K23" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="L23" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="M23" s="52"/>
-      <c r="N23" s="52"/>
-      <c r="O23" s="52"/>
-      <c r="P23" s="52"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="K23" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="L23" s="60" t="s">
+        <v>113</v>
+      </c>
+      <c r="M23" s="60"/>
+      <c r="N23" s="60"/>
+      <c r="O23" s="60"/>
+      <c r="P23" s="60"/>
     </row>
     <row r="24" spans="2:21" ht="13.5" customHeight="1" thickBot="1">
       <c r="B24" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C24" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="52"/>
-      <c r="O24" s="52"/>
-      <c r="P24" s="52"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="K24" s="59"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="60"/>
+      <c r="O24" s="60"/>
+      <c r="P24" s="60"/>
     </row>
     <row r="25" spans="2:21" ht="12.75" customHeight="1" thickTop="1">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
       <c r="K25" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="L25" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="M25" s="54"/>
-      <c r="N25" s="54"/>
-      <c r="O25" s="54"/>
-      <c r="P25" s="54"/>
+        <v>42</v>
+      </c>
+      <c r="L25" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="M25" s="51"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="51"/>
+      <c r="P25" s="51"/>
     </row>
     <row r="26" spans="2:21">
       <c r="B26" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
       <c r="K26" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="L26" s="54" t="s">
-        <v>47</v>
-      </c>
-      <c r="M26" s="54"/>
-      <c r="N26" s="54"/>
-      <c r="O26" s="54"/>
-      <c r="P26" s="54"/>
+        <v>44</v>
+      </c>
+      <c r="L26" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="M26" s="51"/>
+      <c r="N26" s="51"/>
+      <c r="O26" s="51"/>
+      <c r="P26" s="51"/>
     </row>
     <row r="27" spans="2:21">
       <c r="B27" s="12">
@@ -2186,338 +2334,338 @@
       <c r="E27" s="12">
         <v>3</v>
       </c>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
       <c r="K27" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L27" s="54" t="s">
-        <v>118</v>
-      </c>
-      <c r="M27" s="54"/>
-      <c r="N27" s="54"/>
-      <c r="O27" s="54"/>
-      <c r="P27" s="54"/>
+        <v>46</v>
+      </c>
+      <c r="L27" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="M27" s="51"/>
+      <c r="N27" s="51"/>
+      <c r="O27" s="51"/>
+      <c r="P27" s="51"/>
     </row>
     <row r="28" spans="2:21" ht="12.75" customHeight="1">
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="K28" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="L28" s="45"/>
-      <c r="M28" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="N28" s="46"/>
-      <c r="O28" s="46"/>
-      <c r="P28" s="46"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="K28" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="L28" s="59"/>
+      <c r="M28" s="81" t="s">
+        <v>117</v>
+      </c>
+      <c r="N28" s="81"/>
+      <c r="O28" s="81"/>
+      <c r="P28" s="81"/>
     </row>
     <row r="29" spans="2:21">
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
       <c r="H29" s="21"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="45"/>
-      <c r="M29" s="46"/>
-      <c r="N29" s="46"/>
-      <c r="O29" s="46"/>
-      <c r="P29" s="46"/>
+      <c r="K29" s="59"/>
+      <c r="L29" s="59"/>
+      <c r="M29" s="81"/>
+      <c r="N29" s="81"/>
+      <c r="O29" s="81"/>
+      <c r="P29" s="81"/>
     </row>
     <row r="30" spans="2:21" ht="12.75" customHeight="1" thickBot="1">
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="64"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="64"/>
+      <c r="H30" s="64"/>
+      <c r="K30" s="82" t="s">
+        <v>52</v>
+      </c>
+      <c r="L30" s="83" t="s">
+        <v>53</v>
+      </c>
+      <c r="M30" s="83"/>
+      <c r="N30" s="83"/>
+      <c r="O30" s="83"/>
+      <c r="P30" s="83"/>
+    </row>
+    <row r="31" spans="2:21" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B31" s="63"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="64"/>
+      <c r="H31" s="64"/>
+      <c r="K31" s="82"/>
+      <c r="L31" s="83"/>
+      <c r="M31" s="83"/>
+      <c r="N31" s="83"/>
+      <c r="O31" s="83"/>
+      <c r="P31" s="83"/>
+    </row>
+    <row r="32" spans="2:21" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B32" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="K30" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="L30" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
-      <c r="O30" s="48"/>
-      <c r="P30" s="48"/>
-    </row>
-    <row r="31" spans="2:21" ht="13.3" thickTop="1" thickBot="1">
-      <c r="B31" s="27"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="K31" s="47"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="48"/>
-      <c r="N31" s="48"/>
-      <c r="O31" s="48"/>
-      <c r="P31" s="48"/>
-    </row>
-    <row r="32" spans="2:21" ht="13.3" thickTop="1" thickBot="1">
-      <c r="B32" s="13" t="s">
+      <c r="D32" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="E32" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="F32" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="G32" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="H32" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="F32" s="14" t="s">
+    </row>
+    <row r="33" spans="2:16" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B33" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="H33" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="K33" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="L33" s="62"/>
+      <c r="M33" s="62"/>
+      <c r="N33" s="62"/>
+      <c r="O33" s="62"/>
+      <c r="P33" s="62"/>
+    </row>
+    <row r="34" spans="2:16" ht="13.5" thickTop="1">
+      <c r="B34" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="H34" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="K34" s="62"/>
+      <c r="L34" s="62"/>
+      <c r="M34" s="62"/>
+      <c r="N34" s="62"/>
+      <c r="O34" s="62"/>
+      <c r="P34" s="62"/>
+    </row>
+    <row r="35" spans="2:16" ht="12.75" customHeight="1" thickBot="1">
+      <c r="B35" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="73"/>
+      <c r="D35" s="73"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="73"/>
+      <c r="H35" s="74"/>
+      <c r="K35" s="68" t="s">
+        <v>115</v>
+      </c>
+      <c r="L35" s="68"/>
+      <c r="M35" s="68"/>
+      <c r="N35" s="68"/>
+      <c r="O35" s="68"/>
+      <c r="P35" s="68"/>
+    </row>
+    <row r="36" spans="2:16" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B36" s="75"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="76"/>
+      <c r="F36" s="76"/>
+      <c r="G36" s="76"/>
+      <c r="H36" s="77"/>
+      <c r="K36" s="68"/>
+      <c r="L36" s="68"/>
+      <c r="M36" s="68"/>
+      <c r="N36" s="68"/>
+      <c r="O36" s="68"/>
+      <c r="P36" s="68"/>
+    </row>
+    <row r="37" spans="2:16" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B37" s="78"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="79"/>
+      <c r="E37" s="79"/>
+      <c r="F37" s="79"/>
+      <c r="G37" s="79"/>
+      <c r="H37" s="80"/>
+      <c r="K37" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="L37" s="68"/>
+      <c r="M37" s="68"/>
+      <c r="N37" s="68"/>
+      <c r="O37" s="68"/>
+      <c r="P37" s="68"/>
+    </row>
+    <row r="38" spans="2:16" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B38" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G38" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H38" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="K38" s="68"/>
+      <c r="L38" s="68"/>
+      <c r="M38" s="68"/>
+      <c r="N38" s="68"/>
+      <c r="O38" s="68"/>
+      <c r="P38" s="68"/>
+    </row>
+    <row r="39" spans="2:16" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B39" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="G39" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="H32" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="2:16" ht="13.3" thickTop="1" thickBot="1">
-      <c r="B33" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="H33" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="K33" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="L33" s="49"/>
-      <c r="M33" s="49"/>
-      <c r="N33" s="49"/>
-      <c r="O33" s="49"/>
-      <c r="P33" s="49"/>
-    </row>
-    <row r="34" spans="2:16" ht="12.9" thickTop="1">
-      <c r="B34" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E34" s="14" t="s">
+      <c r="H39" s="24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" ht="12.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="K40" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="F34" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="H34" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="K34" s="49"/>
-      <c r="L34" s="49"/>
-      <c r="M34" s="49"/>
-      <c r="N34" s="49"/>
-      <c r="O34" s="49"/>
-      <c r="P34" s="49"/>
-    </row>
-    <row r="35" spans="2:16" ht="12.75" customHeight="1" thickBot="1">
-      <c r="B35" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="38"/>
-      <c r="K35" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="L35" s="32"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="32"/>
-      <c r="O35" s="32"/>
-      <c r="P35" s="32"/>
-    </row>
-    <row r="36" spans="2:16" ht="13.3" thickTop="1" thickBot="1">
-      <c r="B36" s="39"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="41"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
-      <c r="N36" s="32"/>
-      <c r="O36" s="32"/>
-      <c r="P36" s="32"/>
-    </row>
-    <row r="37" spans="2:16" ht="13.3" thickTop="1" thickBot="1">
-      <c r="B37" s="42"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="44"/>
-      <c r="K37" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="L37" s="32"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="32"/>
-      <c r="O37" s="32"/>
-      <c r="P37" s="32"/>
-    </row>
-    <row r="38" spans="2:16" ht="13.3" thickTop="1" thickBot="1">
-      <c r="B38" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G38" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="H38" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="32"/>
-      <c r="N38" s="32"/>
-      <c r="O38" s="32"/>
-      <c r="P38" s="32"/>
-    </row>
-    <row r="39" spans="2:16" ht="13.3" thickTop="1" thickBot="1">
-      <c r="B39" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="H39" s="24" t="s">
+      <c r="L40" s="69"/>
+      <c r="M40" s="69"/>
+      <c r="N40" s="69"/>
+      <c r="O40" s="69"/>
+      <c r="P40" s="69"/>
+    </row>
+    <row r="41" spans="2:16" ht="13.5" thickTop="1">
+      <c r="B41" s="71" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="40" spans="2:16" ht="12.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="K40" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="L40" s="33"/>
-      <c r="M40" s="33"/>
-      <c r="N40" s="33"/>
-      <c r="O40" s="33"/>
-      <c r="P40" s="33"/>
-    </row>
-    <row r="41" spans="2:16" ht="12.9" thickTop="1">
-      <c r="B41" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C41" s="35"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="35"/>
-      <c r="K41" s="33"/>
-      <c r="L41" s="33"/>
-      <c r="M41" s="33"/>
-      <c r="N41" s="33"/>
-      <c r="O41" s="33"/>
-      <c r="P41" s="33"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="71"/>
+      <c r="F41" s="71"/>
+      <c r="G41" s="71"/>
+      <c r="K41" s="69"/>
+      <c r="L41" s="69"/>
+      <c r="M41" s="69"/>
+      <c r="N41" s="69"/>
+      <c r="O41" s="69"/>
+      <c r="P41" s="69"/>
     </row>
     <row r="42" spans="2:16" ht="12.75" customHeight="1">
       <c r="C42" s="15"/>
       <c r="D42" s="15"/>
       <c r="H42" s="15"/>
-      <c r="K42" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="L42" s="34"/>
-      <c r="M42" s="34"/>
-      <c r="N42" s="34"/>
-      <c r="O42" s="34"/>
-      <c r="P42" s="34"/>
+      <c r="K42" s="70" t="s">
+        <v>73</v>
+      </c>
+      <c r="L42" s="70"/>
+      <c r="M42" s="70"/>
+      <c r="N42" s="70"/>
+      <c r="O42" s="70"/>
+      <c r="P42" s="70"/>
     </row>
     <row r="43" spans="2:16">
-      <c r="B43" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="K43" s="34"/>
-      <c r="L43" s="34"/>
-      <c r="M43" s="34"/>
-      <c r="N43" s="34"/>
-      <c r="O43" s="34"/>
-      <c r="P43" s="34"/>
+      <c r="B43" s="66" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="67"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="67"/>
+      <c r="K43" s="70"/>
+      <c r="L43" s="70"/>
+      <c r="M43" s="70"/>
+      <c r="N43" s="70"/>
+      <c r="O43" s="70"/>
+      <c r="P43" s="70"/>
     </row>
     <row r="44" spans="2:16" ht="12.75" customHeight="1">
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="K44" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="L44" s="34"/>
-      <c r="M44" s="34"/>
-      <c r="N44" s="34"/>
-      <c r="O44" s="34"/>
-      <c r="P44" s="34"/>
+      <c r="B44" s="67"/>
+      <c r="C44" s="67"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="67"/>
+      <c r="F44" s="67"/>
+      <c r="G44" s="67"/>
+      <c r="K44" s="70" t="s">
+        <v>84</v>
+      </c>
+      <c r="L44" s="70"/>
+      <c r="M44" s="70"/>
+      <c r="N44" s="70"/>
+      <c r="O44" s="70"/>
+      <c r="P44" s="70"/>
     </row>
     <row r="45" spans="2:16">
       <c r="B45" s="22"/>
@@ -2526,12 +2674,12 @@
       <c r="E45" s="22"/>
       <c r="F45" s="22"/>
       <c r="G45" s="22"/>
-      <c r="K45" s="34"/>
-      <c r="L45" s="34"/>
-      <c r="M45" s="34"/>
-      <c r="N45" s="34"/>
-      <c r="O45" s="34"/>
-      <c r="P45" s="34"/>
+      <c r="K45" s="70"/>
+      <c r="L45" s="70"/>
+      <c r="M45" s="70"/>
+      <c r="N45" s="70"/>
+      <c r="O45" s="70"/>
+      <c r="P45" s="70"/>
     </row>
     <row r="46" spans="2:16">
       <c r="B46" s="22"/>
@@ -2540,12 +2688,12 @@
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
       <c r="G46" s="22"/>
-      <c r="K46" s="34"/>
-      <c r="L46" s="34"/>
-      <c r="M46" s="34"/>
-      <c r="N46" s="34"/>
-      <c r="O46" s="34"/>
-      <c r="P46" s="34"/>
+      <c r="K46" s="70"/>
+      <c r="L46" s="70"/>
+      <c r="M46" s="70"/>
+      <c r="N46" s="70"/>
+      <c r="O46" s="70"/>
+      <c r="P46" s="70"/>
     </row>
     <row r="47" spans="2:16">
       <c r="B47" s="22"/>
@@ -2554,12 +2702,12 @@
       <c r="E47" s="22"/>
       <c r="F47" s="22"/>
       <c r="G47" s="22"/>
-      <c r="K47" s="34"/>
-      <c r="L47" s="34"/>
-      <c r="M47" s="34"/>
-      <c r="N47" s="34"/>
-      <c r="O47" s="34"/>
-      <c r="P47" s="34"/>
+      <c r="K47" s="70"/>
+      <c r="L47" s="70"/>
+      <c r="M47" s="70"/>
+      <c r="N47" s="70"/>
+      <c r="O47" s="70"/>
+      <c r="P47" s="70"/>
     </row>
     <row r="48" spans="2:16">
       <c r="B48" s="22"/>
@@ -2569,80 +2717,80 @@
       <c r="F48" s="22"/>
       <c r="G48" s="22"/>
       <c r="K48" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="L48" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="M48" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="L48" s="19" t="s">
+      <c r="N48" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="M48" s="19" t="s">
+      <c r="O48" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="N48" s="19" t="s">
+      <c r="P48" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="O48" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="P48" s="20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49" spans="2:16" ht="12.9" thickBot="1">
+    </row>
+    <row r="49" spans="2:16" ht="13.5" thickBot="1">
       <c r="B49" s="22"/>
       <c r="C49" s="22"/>
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
       <c r="F49" s="22"/>
       <c r="G49" s="22"/>
-      <c r="K49" s="29" t="s">
+      <c r="K49" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L49" s="65"/>
+      <c r="M49" s="65"/>
+      <c r="N49" s="65"/>
+      <c r="O49" s="65"/>
+      <c r="P49" s="65"/>
+    </row>
+    <row r="50" spans="2:16" ht="13.5" thickTop="1"/>
+    <row r="51" spans="2:16">
+      <c r="K51" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="L49" s="29"/>
-      <c r="M49" s="29"/>
-      <c r="N49" s="29"/>
-      <c r="O49" s="29"/>
-      <c r="P49" s="29"/>
-    </row>
-    <row r="50" spans="2:16" ht="12.9" thickTop="1"/>
-    <row r="51" spans="2:16">
-      <c r="K51" s="83" t="s">
+      <c r="L51" s="25"/>
+      <c r="M51" s="25"/>
+      <c r="N51" s="25"/>
+      <c r="O51" s="25"/>
+      <c r="P51" s="25"/>
+    </row>
+    <row r="52" spans="2:16">
+      <c r="K52" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="L52" s="25"/>
+      <c r="M52" s="25"/>
+      <c r="N52" s="25"/>
+      <c r="O52" s="25"/>
+      <c r="P52" s="25"/>
+    </row>
+    <row r="53" spans="2:16">
+      <c r="K53" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="L51" s="75"/>
-      <c r="M51" s="75"/>
-      <c r="N51" s="75"/>
-      <c r="O51" s="75"/>
-      <c r="P51" s="75"/>
-    </row>
-    <row r="52" spans="2:16">
-      <c r="K52" s="75" t="s">
+      <c r="L53" s="25"/>
+      <c r="M53" s="25"/>
+      <c r="N53" s="25"/>
+      <c r="O53" s="25"/>
+      <c r="P53" s="25"/>
+    </row>
+    <row r="54" spans="2:16">
+      <c r="K54" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="L52" s="75"/>
-      <c r="M52" s="75"/>
-      <c r="N52" s="75"/>
-      <c r="O52" s="75"/>
-      <c r="P52" s="75"/>
-    </row>
-    <row r="53" spans="2:16">
-      <c r="K53" s="75" t="s">
-        <v>98</v>
-      </c>
-      <c r="L53" s="75"/>
-      <c r="M53" s="75"/>
-      <c r="N53" s="75"/>
-      <c r="O53" s="75"/>
-      <c r="P53" s="75"/>
-    </row>
-    <row r="54" spans="2:16">
-      <c r="K54" s="75" t="s">
-        <v>99</v>
-      </c>
-      <c r="L54" s="75"/>
-      <c r="M54" s="75"/>
-      <c r="N54" s="75"/>
-      <c r="O54" s="75"/>
-      <c r="P54" s="75"/>
+      <c r="L54" s="25"/>
+      <c r="M54" s="25"/>
+      <c r="N54" s="25"/>
+      <c r="O54" s="25"/>
+      <c r="P54" s="25"/>
     </row>
     <row r="55" spans="2:16">
       <c r="C55" s="15"/>
@@ -2707,6 +2855,58 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="68">
+    <mergeCell ref="B30:H31"/>
+    <mergeCell ref="K49:P49"/>
+    <mergeCell ref="B43:G44"/>
+    <mergeCell ref="K35:P38"/>
+    <mergeCell ref="K40:P41"/>
+    <mergeCell ref="K42:P43"/>
+    <mergeCell ref="K44:P47"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B35:H37"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L30:P31"/>
+    <mergeCell ref="K33:P34"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:P18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="F16:H21"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="L23:P24"/>
+    <mergeCell ref="B21:E23"/>
+    <mergeCell ref="F23:H28"/>
+    <mergeCell ref="K28:L29"/>
+    <mergeCell ref="M28:P29"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:P15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:P16"/>
+    <mergeCell ref="B16:E17"/>
+    <mergeCell ref="F10:H14"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="K8:L9"/>
+    <mergeCell ref="M8:P9"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:H8"/>
+    <mergeCell ref="B9:E10"/>
+    <mergeCell ref="K11:P12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:P14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B3:E4"/>
+    <mergeCell ref="F3:H5"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:P7"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="K53:P53"/>
     <mergeCell ref="K54:P54"/>
     <mergeCell ref="K2:P3"/>
@@ -2720,61 +2920,9 @@
     <mergeCell ref="M22:P22"/>
     <mergeCell ref="K51:P51"/>
     <mergeCell ref="K52:P52"/>
-    <mergeCell ref="B3:E4"/>
-    <mergeCell ref="F3:H5"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:P7"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F10:H14"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="K8:L9"/>
-    <mergeCell ref="M8:P9"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:H8"/>
-    <mergeCell ref="B9:E10"/>
-    <mergeCell ref="K11:P12"/>
     <mergeCell ref="L25:P25"/>
     <mergeCell ref="L26:P26"/>
     <mergeCell ref="L27:P27"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:P14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:P15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:P16"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:P20"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="L23:P24"/>
-    <mergeCell ref="B21:E23"/>
-    <mergeCell ref="B16:E17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:P18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="F16:H21"/>
-    <mergeCell ref="F23:H28"/>
-    <mergeCell ref="B30:H31"/>
-    <mergeCell ref="K49:P49"/>
-    <mergeCell ref="B43:G44"/>
-    <mergeCell ref="K35:P38"/>
-    <mergeCell ref="K40:P41"/>
-    <mergeCell ref="K42:P43"/>
-    <mergeCell ref="K44:P47"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B35:H37"/>
-    <mergeCell ref="K28:L29"/>
-    <mergeCell ref="M28:P29"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="L30:P31"/>
-    <mergeCell ref="K33:P34"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" fitToWidth="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>